<commit_message>
replace DT with knitr::kable
</commit_message>
<xml_diff>
--- a/data/Tables.xlsx
+++ b/data/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GitHub/borderlands/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/borderlands/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F55D21A0-B8F4-0646-B3B2-D1E2FFE09DE2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C592191-641F-BF43-B833-C69C886C79D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16620" xr2:uid="{188CABF9-3390-E543-97E1-F37DF5D8587E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Сегменты границы России</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Северо-Западный</t>
-  </si>
-  <si>
-    <t>2 420,5*</t>
   </si>
   <si>
     <t>Калининградский</t>
@@ -557,13 +554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DC3DFA-1BE7-1D4C-862A-0371094C6B02}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="106" thickTop="1" thickBot="1">
+    <row r="1" spans="1:7" ht="100" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +613,8 @@
       <c r="B3" s="5">
         <v>737.3</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
+      <c r="C3" s="9">
+        <v>2420.5</v>
       </c>
       <c r="D3" s="6">
         <v>17.3</v>
@@ -634,7 +631,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" thickBot="1">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5">
         <v>524.70000000000005</v>
@@ -657,7 +654,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
         <v>1239</v>
@@ -680,7 +677,7 @@
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5">
         <v>2245.8000000000002</v>
@@ -703,7 +700,7 @@
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5">
         <v>1247.9000000000001</v>
@@ -726,7 +723,7 @@
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5">
         <v>7598.6</v>
@@ -749,7 +746,7 @@
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5">
         <v>3485</v>
@@ -772,7 +769,7 @@
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11">
         <v>4209.3</v>

</xml_diff>